<commit_message>
it is not mandatory to fill all the boxes
</commit_message>
<xml_diff>
--- a/public/templates/template.xlsx
+++ b/public/templates/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soufiane.Erradi\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8186D8B-B09A-4404-BB1D-8B4D4763AFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56631D6-5B77-4A3D-ACDE-1888A95799A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{35161D93-A83C-4741-B992-1D554621739D}"/>
+    <workbookView xWindow="34365" yWindow="180" windowWidth="21600" windowHeight="15420" xr2:uid="{35161D93-A83C-4741-B992-1D554621739D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
     <t>Company:</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>iRed Service Options</t>
-  </si>
-  <si>
-    <t>Comment</t>
   </si>
   <si>
     <t>Comments</t>
@@ -274,7 +271,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -575,6 +572,17 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -621,16 +629,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -671,10 +673,106 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -683,107 +781,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1121,8 +1129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5F62A0-21B3-4BE8-8A16-29D4D519CB27}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25:P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,584 +1144,582 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
-        <v>36</v>
+      <c r="A1" s="54" t="s">
+        <v>35</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="69" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="70"/>
+      <c r="F1" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="48" t="s">
+      <c r="G1" s="47"/>
+      <c r="H1" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="49"/>
-      <c r="H1" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="43"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="45" t="s">
+      <c r="I1" s="41"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="42" t="s">
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="43"/>
-      <c r="P1" s="44"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="42"/>
     </row>
     <row r="2" spans="1:16" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="70"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="36"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="34"/>
       <c r="D2" s="37"/>
-      <c r="E2" s="38"/>
+      <c r="E2" s="39"/>
       <c r="F2" s="37"/>
-      <c r="G2" s="38"/>
+      <c r="G2" s="39"/>
       <c r="H2" s="37"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="47"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="45"/>
       <c r="M2" s="37"/>
       <c r="N2" s="37"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="39"/>
     </row>
     <row r="3" spans="1:16" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="71"/>
-      <c r="B3" s="19" t="s">
+      <c r="A3" s="56"/>
+      <c r="B3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="36"/>
+      <c r="D3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-    </row>
-    <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="66" t="s">
+      <c r="C4" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="60"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="62"/>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="52"/>
+      <c r="B5" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="63"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="64"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="65"/>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="52"/>
+      <c r="B6" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="63"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="64"/>
+      <c r="O6" s="64"/>
+      <c r="P6" s="65"/>
+    </row>
+    <row r="7" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="52"/>
+      <c r="B7" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="63"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="64"/>
+      <c r="N7" s="64"/>
+      <c r="O7" s="64"/>
+      <c r="P7" s="65"/>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="53"/>
+      <c r="B8" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="66"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="67"/>
+      <c r="P8" s="68"/>
+    </row>
+    <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="52"/>
-    </row>
-    <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="67"/>
-      <c r="B5" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="53"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="54"/>
-      <c r="M5" s="54"/>
-      <c r="N5" s="54"/>
-      <c r="O5" s="54"/>
-      <c r="P5" s="55"/>
-    </row>
-    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="67"/>
-      <c r="B6" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="53"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="54"/>
-      <c r="P6" s="55"/>
-    </row>
-    <row r="7" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="67"/>
-      <c r="B7" s="21" t="s">
+      <c r="B9" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="60"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="61"/>
+      <c r="O9" s="61"/>
+      <c r="P9" s="62"/>
+    </row>
+    <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="58"/>
+      <c r="B10" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="63"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="64"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="64"/>
+      <c r="M10" s="64"/>
+      <c r="N10" s="64"/>
+      <c r="O10" s="64"/>
+      <c r="P10" s="65"/>
+    </row>
+    <row r="11" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="59"/>
+      <c r="B11" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="66"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="67"/>
+      <c r="N11" s="67"/>
+      <c r="O11" s="67"/>
+      <c r="P11" s="68"/>
+    </row>
+    <row r="12" spans="1:16" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="54"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="54"/>
-      <c r="P7" s="55"/>
-    </row>
-    <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="68"/>
-      <c r="B8" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="56"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="57"/>
-      <c r="K8" s="57"/>
-      <c r="L8" s="57"/>
-      <c r="M8" s="57"/>
-      <c r="N8" s="57"/>
-      <c r="O8" s="57"/>
-      <c r="P8" s="58"/>
-    </row>
-    <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="72" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="51"/>
-      <c r="O9" s="51"/>
-      <c r="P9" s="52"/>
-    </row>
-    <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="73"/>
-      <c r="B10" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="53"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="54"/>
-      <c r="M10" s="54"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="54"/>
-      <c r="P10" s="55"/>
-    </row>
-    <row r="11" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="74"/>
-      <c r="B11" s="29" t="s">
+      <c r="C12" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="60"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="61"/>
+      <c r="M12" s="61"/>
+      <c r="N12" s="61"/>
+      <c r="O12" s="61"/>
+      <c r="P12" s="62"/>
+    </row>
+    <row r="13" spans="1:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="58"/>
+      <c r="B13" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="63"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="64"/>
+      <c r="L13" s="64"/>
+      <c r="M13" s="64"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="64"/>
+      <c r="P13" s="65"/>
+    </row>
+    <row r="14" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="58"/>
+      <c r="B14" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="63"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="64"/>
+      <c r="I14" s="64"/>
+      <c r="J14" s="64"/>
+      <c r="K14" s="64"/>
+      <c r="L14" s="64"/>
+      <c r="M14" s="64"/>
+      <c r="N14" s="64"/>
+      <c r="O14" s="64"/>
+      <c r="P14" s="65"/>
+    </row>
+    <row r="15" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="58"/>
+      <c r="B15" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="66"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="67"/>
+      <c r="M15" s="67"/>
+      <c r="N15" s="67"/>
+      <c r="O15" s="67"/>
+      <c r="P15" s="68"/>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="58"/>
+      <c r="B16" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="60"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="61"/>
+      <c r="L16" s="61"/>
+      <c r="M16" s="61"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="61"/>
+      <c r="P16" s="62"/>
+    </row>
+    <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="58"/>
+      <c r="B17" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="56"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="57"/>
-      <c r="N11" s="57"/>
-      <c r="O11" s="57"/>
-      <c r="P11" s="58"/>
-    </row>
-    <row r="12" spans="1:16" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="72" t="s">
+      <c r="C17" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="63"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="64"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="64"/>
+      <c r="M17" s="64"/>
+      <c r="N17" s="64"/>
+      <c r="O17" s="64"/>
+      <c r="P17" s="65"/>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="59"/>
+      <c r="B18" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="66"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="67"/>
+      <c r="M18" s="67"/>
+      <c r="N18" s="67"/>
+      <c r="O18" s="67"/>
+      <c r="P18" s="68"/>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B19" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="60"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="61"/>
+      <c r="J19" s="61"/>
+      <c r="K19" s="61"/>
+      <c r="L19" s="61"/>
+      <c r="M19" s="61"/>
+      <c r="N19" s="61"/>
+      <c r="O19" s="61"/>
+      <c r="P19" s="62"/>
+    </row>
+    <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="49"/>
+      <c r="B20" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="63"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="64"/>
+      <c r="H20" s="64"/>
+      <c r="I20" s="64"/>
+      <c r="J20" s="64"/>
+      <c r="K20" s="64"/>
+      <c r="L20" s="64"/>
+      <c r="M20" s="64"/>
+      <c r="N20" s="64"/>
+      <c r="O20" s="64"/>
+      <c r="P20" s="65"/>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="49"/>
+      <c r="B21" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="63"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="64"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="64"/>
+      <c r="M21" s="64"/>
+      <c r="N21" s="64"/>
+      <c r="O21" s="64"/>
+      <c r="P21" s="65"/>
+    </row>
+    <row r="22" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="49"/>
+      <c r="B22" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="63"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="64"/>
+      <c r="I22" s="64"/>
+      <c r="J22" s="64"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="64"/>
+      <c r="M22" s="64"/>
+      <c r="N22" s="64"/>
+      <c r="O22" s="64"/>
+      <c r="P22" s="65"/>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="50"/>
+      <c r="B23" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="66"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="67"/>
+      <c r="M23" s="67"/>
+      <c r="N23" s="67"/>
+      <c r="O23" s="67"/>
+      <c r="P23" s="68"/>
+    </row>
+    <row r="24" spans="1:16" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="51"/>
-      <c r="N12" s="51"/>
-      <c r="O12" s="51"/>
-      <c r="P12" s="52"/>
-    </row>
-    <row r="13" spans="1:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="73"/>
-      <c r="B13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="53"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="54"/>
-      <c r="M13" s="54"/>
-      <c r="N13" s="54"/>
-      <c r="O13" s="54"/>
-      <c r="P13" s="55"/>
-    </row>
-    <row r="14" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="73"/>
-      <c r="B14" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="53"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="54"/>
-      <c r="O14" s="54"/>
-      <c r="P14" s="55"/>
-    </row>
-    <row r="15" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="73"/>
-      <c r="B15" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="56"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="57"/>
-      <c r="L15" s="57"/>
-      <c r="M15" s="57"/>
-      <c r="N15" s="57"/>
-      <c r="O15" s="57"/>
-      <c r="P15" s="58"/>
-    </row>
-    <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="73"/>
-      <c r="B16" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="51"/>
-      <c r="M16" s="51"/>
-      <c r="N16" s="51"/>
-      <c r="O16" s="51"/>
-      <c r="P16" s="52"/>
-    </row>
-    <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="73"/>
-      <c r="B17" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="53"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="54"/>
-      <c r="L17" s="54"/>
-      <c r="M17" s="54"/>
-      <c r="N17" s="54"/>
-      <c r="O17" s="54"/>
-      <c r="P17" s="55"/>
-    </row>
-    <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="74"/>
-      <c r="B18" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="56"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="57"/>
-      <c r="M18" s="57"/>
-      <c r="N18" s="57"/>
-      <c r="O18" s="57"/>
-      <c r="P18" s="58"/>
-    </row>
-    <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="64" t="s">
+      <c r="C24" s="31"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="72"/>
+      <c r="I24" s="72"/>
+      <c r="J24" s="72"/>
+      <c r="K24" s="72"/>
+      <c r="L24" s="72"/>
+      <c r="M24" s="72"/>
+      <c r="N24" s="72"/>
+      <c r="O24" s="72"/>
+      <c r="P24" s="73"/>
+    </row>
+    <row r="25" spans="1:16" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="74"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="72"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="72"/>
+      <c r="J25" s="72"/>
+      <c r="K25" s="72"/>
+      <c r="L25" s="72"/>
+      <c r="M25" s="72"/>
+      <c r="N25" s="72"/>
+      <c r="O25" s="72"/>
+      <c r="P25" s="73"/>
+    </row>
+    <row r="26" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="50"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="51"/>
-      <c r="P19" s="52"/>
-    </row>
-    <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="64"/>
-      <c r="B20" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="53"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="54"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="54"/>
-      <c r="K20" s="54"/>
-      <c r="L20" s="54"/>
-      <c r="M20" s="54"/>
-      <c r="N20" s="54"/>
-      <c r="O20" s="54"/>
-      <c r="P20" s="55"/>
-    </row>
-    <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="64"/>
-      <c r="B21" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="53"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="54"/>
-      <c r="N21" s="54"/>
-      <c r="O21" s="54"/>
-      <c r="P21" s="55"/>
-    </row>
-    <row r="22" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="64"/>
-      <c r="B22" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="53"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="54"/>
-      <c r="L22" s="54"/>
-      <c r="M22" s="54"/>
-      <c r="N22" s="54"/>
-      <c r="O22" s="54"/>
-      <c r="P22" s="55"/>
-    </row>
-    <row r="23" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="65"/>
-      <c r="B23" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="56"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="57"/>
-      <c r="J23" s="57"/>
-      <c r="K23" s="57"/>
-      <c r="L23" s="57"/>
-      <c r="M23" s="57"/>
-      <c r="N23" s="57"/>
-      <c r="O23" s="57"/>
-      <c r="P23" s="58"/>
-    </row>
-    <row r="24" spans="1:16" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="60"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="60"/>
-      <c r="H24" s="60"/>
-      <c r="I24" s="60"/>
-      <c r="J24" s="60"/>
-      <c r="K24" s="60"/>
-      <c r="L24" s="60"/>
-      <c r="M24" s="60"/>
-      <c r="N24" s="60"/>
-      <c r="O24" s="60"/>
-      <c r="P24" s="61"/>
-    </row>
-    <row r="25" spans="1:16" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="62"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="60"/>
-      <c r="H25" s="60"/>
-      <c r="I25" s="60"/>
-      <c r="J25" s="60"/>
-      <c r="K25" s="60"/>
-      <c r="L25" s="60"/>
-      <c r="M25" s="60"/>
-      <c r="N25" s="60"/>
-      <c r="O25" s="60"/>
-      <c r="P25" s="61"/>
-    </row>
-    <row r="26" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="63" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D26" s="12">
         <v>1</v>
@@ -1752,15 +1758,15 @@
         <v>12</v>
       </c>
       <c r="P26" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="64"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
+      <c r="A27" s="49"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
@@ -1771,14 +1777,14 @@
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
       <c r="O27" s="8"/>
-      <c r="P27" s="26"/>
+      <c r="P27" s="24"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="64"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
+      <c r="A28" s="49"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
@@ -1789,14 +1795,14 @@
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
       <c r="O28" s="8"/>
-      <c r="P28" s="26"/>
+      <c r="P28" s="24"/>
     </row>
     <row r="29" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="64"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
+      <c r="A29" s="49"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
@@ -1807,10 +1813,10 @@
       <c r="M29" s="8"/>
       <c r="N29" s="8"/>
       <c r="O29" s="8"/>
-      <c r="P29" s="26"/>
+      <c r="P29" s="24"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="64"/>
+      <c r="A30" s="49"/>
       <c r="B30" s="2"/>
       <c r="C30" s="4"/>
       <c r="D30" s="5"/>
@@ -1828,7 +1834,7 @@
       <c r="P30" s="7"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="64"/>
+      <c r="A31" s="49"/>
       <c r="B31" s="4"/>
       <c r="C31" s="9"/>
       <c r="D31" s="5"/>
@@ -1846,7 +1852,7 @@
       <c r="P31" s="7"/>
     </row>
     <row r="32" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="64"/>
+      <c r="A32" s="49"/>
       <c r="B32" s="9"/>
       <c r="C32" s="4"/>
       <c r="D32" s="5"/>
@@ -1864,7 +1870,7 @@
       <c r="P32" s="7"/>
     </row>
     <row r="33" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="64"/>
+      <c r="A33" s="49"/>
       <c r="B33" s="2"/>
       <c r="C33" s="4"/>
       <c r="D33" s="5"/>
@@ -1882,7 +1888,7 @@
       <c r="P33" s="7"/>
     </row>
     <row r="34" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="64"/>
+      <c r="A34" s="49"/>
       <c r="B34" s="2"/>
       <c r="C34" s="4"/>
       <c r="D34" s="5"/>
@@ -1900,7 +1906,7 @@
       <c r="P34" s="7"/>
     </row>
     <row r="35" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="64"/>
+      <c r="A35" s="49"/>
       <c r="B35" s="2"/>
       <c r="C35" s="4"/>
       <c r="D35" s="5"/>
@@ -1918,7 +1924,7 @@
       <c r="P35" s="7"/>
     </row>
     <row r="36" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="65"/>
+      <c r="A36" s="50"/>
       <c r="B36" s="2"/>
       <c r="C36" s="4"/>
       <c r="D36" s="5"/>
@@ -1953,7 +1959,7 @@
       <c r="P37" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="25">
     <mergeCell ref="A26:A36"/>
     <mergeCell ref="A4:A8"/>
     <mergeCell ref="D3:P3"/>
@@ -1970,6 +1976,7 @@
     <mergeCell ref="D16:P18"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B3:C3"/>
     <mergeCell ref="N2:P2"/>
     <mergeCell ref="N1:P1"/>
     <mergeCell ref="K1:M1"/>

</xml_diff>

<commit_message>
use the same logic you are using with the rest of the fields with the ba
</commit_message>
<xml_diff>
--- a/public/templates/template.xlsx
+++ b/public/templates/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soufiane.Erradi\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56631D6-5B77-4A3D-ACDE-1888A95799A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC21605C-1E85-407F-88B0-FA8A007FC1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34365" yWindow="180" windowWidth="21600" windowHeight="15420" xr2:uid="{35161D93-A83C-4741-B992-1D554621739D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{35161D93-A83C-4741-B992-1D554621739D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
   <si>
     <t>Company:</t>
   </si>
@@ -775,23 +775,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1127,10 +1127,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5F62A0-21B3-4BE8-8A16-29D4D519CB27}">
-  <dimension ref="A1:P37"/>
+  <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25:P25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,11 +1139,11 @@
     <col min="2" max="2" width="30.140625" customWidth="1"/>
     <col min="3" max="3" width="36.5703125" customWidth="1"/>
     <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="14" max="15" width="9.140625" customWidth="1"/>
-    <col min="16" max="16" width="9" customWidth="1"/>
+    <col min="14" max="16" width="9.140625" customWidth="1"/>
+    <col min="17" max="17" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>35</v>
       </c>
@@ -1153,10 +1153,10 @@
       <c r="C1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="70"/>
+      <c r="E1" s="74"/>
       <c r="F1" s="46" t="s">
         <v>41</v>
       </c>
@@ -1175,9 +1175,10 @@
         <v>3</v>
       </c>
       <c r="O1" s="41"/>
-      <c r="P1" s="42"/>
-    </row>
-    <row r="2" spans="1:16" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P1" s="41"/>
+      <c r="Q1" s="42"/>
+    </row>
+    <row r="2" spans="1:17" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="55"/>
       <c r="B2" s="22"/>
       <c r="C2" s="34"/>
@@ -1193,9 +1194,10 @@
       <c r="M2" s="37"/>
       <c r="N2" s="37"/>
       <c r="O2" s="38"/>
-      <c r="P2" s="39"/>
-    </row>
-    <row r="3" spans="1:16" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P2" s="38"/>
+      <c r="Q2" s="39"/>
+    </row>
+    <row r="3" spans="1:17" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="56"/>
       <c r="B3" s="35" t="s">
         <v>4</v>
@@ -1216,8 +1218,9 @@
       <c r="N3" s="43"/>
       <c r="O3" s="43"/>
       <c r="P3" s="43"/>
-    </row>
-    <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q3" s="43"/>
+    </row>
+    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>30</v>
       </c>
@@ -1239,9 +1242,10 @@
       <c r="M4" s="61"/>
       <c r="N4" s="61"/>
       <c r="O4" s="61"/>
-      <c r="P4" s="62"/>
-    </row>
-    <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P4" s="61"/>
+      <c r="Q4" s="62"/>
+    </row>
+    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="52"/>
       <c r="B5" s="19" t="s">
         <v>7</v>
@@ -1261,9 +1265,10 @@
       <c r="M5" s="64"/>
       <c r="N5" s="64"/>
       <c r="O5" s="64"/>
-      <c r="P5" s="65"/>
-    </row>
-    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P5" s="64"/>
+      <c r="Q5" s="65"/>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="52"/>
       <c r="B6" s="19" t="s">
         <v>8</v>
@@ -1283,9 +1288,10 @@
       <c r="M6" s="64"/>
       <c r="N6" s="64"/>
       <c r="O6" s="64"/>
-      <c r="P6" s="65"/>
-    </row>
-    <row r="7" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P6" s="64"/>
+      <c r="Q6" s="65"/>
+    </row>
+    <row r="7" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="52"/>
       <c r="B7" s="20" t="s">
         <v>9</v>
@@ -1305,9 +1311,10 @@
       <c r="M7" s="64"/>
       <c r="N7" s="64"/>
       <c r="O7" s="64"/>
-      <c r="P7" s="65"/>
-    </row>
-    <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P7" s="64"/>
+      <c r="Q7" s="65"/>
+    </row>
+    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="53"/>
       <c r="B8" s="19" t="s">
         <v>29</v>
@@ -1327,9 +1334,10 @@
       <c r="M8" s="67"/>
       <c r="N8" s="67"/>
       <c r="O8" s="67"/>
-      <c r="P8" s="68"/>
-    </row>
-    <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P8" s="67"/>
+      <c r="Q8" s="68"/>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="57" t="s">
         <v>31</v>
       </c>
@@ -1351,9 +1359,10 @@
       <c r="M9" s="61"/>
       <c r="N9" s="61"/>
       <c r="O9" s="61"/>
-      <c r="P9" s="62"/>
-    </row>
-    <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P9" s="61"/>
+      <c r="Q9" s="62"/>
+    </row>
+    <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="58"/>
       <c r="B10" s="26" t="s">
         <v>16</v>
@@ -1373,9 +1382,10 @@
       <c r="M10" s="64"/>
       <c r="N10" s="64"/>
       <c r="O10" s="64"/>
-      <c r="P10" s="65"/>
-    </row>
-    <row r="11" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P10" s="64"/>
+      <c r="Q10" s="65"/>
+    </row>
+    <row r="11" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="59"/>
       <c r="B11" s="27" t="s">
         <v>17</v>
@@ -1395,9 +1405,10 @@
       <c r="M11" s="67"/>
       <c r="N11" s="67"/>
       <c r="O11" s="67"/>
-      <c r="P11" s="68"/>
-    </row>
-    <row r="12" spans="1:16" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P11" s="67"/>
+      <c r="Q11" s="68"/>
+    </row>
+    <row r="12" spans="1:17" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="57" t="s">
         <v>32</v>
       </c>
@@ -1419,9 +1430,10 @@
       <c r="M12" s="61"/>
       <c r="N12" s="61"/>
       <c r="O12" s="61"/>
-      <c r="P12" s="62"/>
-    </row>
-    <row r="13" spans="1:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P12" s="61"/>
+      <c r="Q12" s="62"/>
+    </row>
+    <row r="13" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="58"/>
       <c r="B13" s="29" t="s">
         <v>21</v>
@@ -1441,9 +1453,10 @@
       <c r="M13" s="64"/>
       <c r="N13" s="64"/>
       <c r="O13" s="64"/>
-      <c r="P13" s="65"/>
-    </row>
-    <row r="14" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P13" s="64"/>
+      <c r="Q13" s="65"/>
+    </row>
+    <row r="14" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="58"/>
       <c r="B14" s="30" t="s">
         <v>22</v>
@@ -1463,9 +1476,10 @@
       <c r="M14" s="64"/>
       <c r="N14" s="64"/>
       <c r="O14" s="64"/>
-      <c r="P14" s="65"/>
-    </row>
-    <row r="15" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P14" s="64"/>
+      <c r="Q14" s="65"/>
+    </row>
+    <row r="15" spans="1:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="58"/>
       <c r="B15" s="30" t="s">
         <v>23</v>
@@ -1485,9 +1499,10 @@
       <c r="M15" s="67"/>
       <c r="N15" s="67"/>
       <c r="O15" s="67"/>
-      <c r="P15" s="68"/>
-    </row>
-    <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P15" s="67"/>
+      <c r="Q15" s="68"/>
+    </row>
+    <row r="16" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="58"/>
       <c r="B16" s="26" t="s">
         <v>19</v>
@@ -1507,9 +1522,10 @@
       <c r="M16" s="61"/>
       <c r="N16" s="61"/>
       <c r="O16" s="61"/>
-      <c r="P16" s="62"/>
-    </row>
-    <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P16" s="61"/>
+      <c r="Q16" s="62"/>
+    </row>
+    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="58"/>
       <c r="B17" s="26" t="s">
         <v>18</v>
@@ -1529,9 +1545,10 @@
       <c r="M17" s="64"/>
       <c r="N17" s="64"/>
       <c r="O17" s="64"/>
-      <c r="P17" s="65"/>
-    </row>
-    <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P17" s="64"/>
+      <c r="Q17" s="65"/>
+    </row>
+    <row r="18" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="59"/>
       <c r="B18" s="26" t="s">
         <v>20</v>
@@ -1551,9 +1568,10 @@
       <c r="M18" s="67"/>
       <c r="N18" s="67"/>
       <c r="O18" s="67"/>
-      <c r="P18" s="68"/>
-    </row>
-    <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P18" s="67"/>
+      <c r="Q18" s="68"/>
+    </row>
+    <row r="19" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="49" t="s">
         <v>33</v>
       </c>
@@ -1575,9 +1593,10 @@
       <c r="M19" s="61"/>
       <c r="N19" s="61"/>
       <c r="O19" s="61"/>
-      <c r="P19" s="62"/>
-    </row>
-    <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P19" s="61"/>
+      <c r="Q19" s="62"/>
+    </row>
+    <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="49"/>
       <c r="B20" s="26" t="s">
         <v>25</v>
@@ -1597,9 +1616,10 @@
       <c r="M20" s="64"/>
       <c r="N20" s="64"/>
       <c r="O20" s="64"/>
-      <c r="P20" s="65"/>
-    </row>
-    <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P20" s="64"/>
+      <c r="Q20" s="65"/>
+    </row>
+    <row r="21" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="49"/>
       <c r="B21" s="26" t="s">
         <v>26</v>
@@ -1619,9 +1639,10 @@
       <c r="M21" s="64"/>
       <c r="N21" s="64"/>
       <c r="O21" s="64"/>
-      <c r="P21" s="65"/>
-    </row>
-    <row r="22" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P21" s="64"/>
+      <c r="Q21" s="65"/>
+    </row>
+    <row r="22" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="49"/>
       <c r="B22" s="27" t="s">
         <v>27</v>
@@ -1641,9 +1662,10 @@
       <c r="M22" s="64"/>
       <c r="N22" s="64"/>
       <c r="O22" s="64"/>
-      <c r="P22" s="65"/>
-    </row>
-    <row r="23" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P22" s="64"/>
+      <c r="Q22" s="65"/>
+    </row>
+    <row r="23" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="50"/>
       <c r="B23" s="27" t="s">
         <v>28</v>
@@ -1663,31 +1685,35 @@
       <c r="M23" s="67"/>
       <c r="N23" s="67"/>
       <c r="O23" s="67"/>
-      <c r="P23" s="68"/>
-    </row>
-    <row r="24" spans="1:16" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="P23" s="67"/>
+      <c r="Q23" s="68"/>
+    </row>
+    <row r="24" spans="1:17" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
         <v>36</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="71"/>
-      <c r="E24" s="72"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="72"/>
-      <c r="H24" s="72"/>
-      <c r="I24" s="72"/>
-      <c r="J24" s="72"/>
-      <c r="K24" s="72"/>
-      <c r="L24" s="72"/>
-      <c r="M24" s="72"/>
-      <c r="N24" s="72"/>
-      <c r="O24" s="72"/>
-      <c r="P24" s="73"/>
-    </row>
-    <row r="25" spans="1:16" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="69"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="70"/>
+      <c r="J24" s="70"/>
+      <c r="K24" s="70"/>
+      <c r="L24" s="70"/>
+      <c r="M24" s="70"/>
+      <c r="N24" s="70"/>
+      <c r="O24" s="70"/>
+      <c r="P24" s="70"/>
+      <c r="Q24" s="71"/>
+    </row>
+    <row r="25" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
         <v>37</v>
       </c>
@@ -1697,21 +1723,22 @@
       <c r="C25" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="74"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="72"/>
-      <c r="H25" s="72"/>
-      <c r="I25" s="72"/>
-      <c r="J25" s="72"/>
-      <c r="K25" s="72"/>
-      <c r="L25" s="72"/>
-      <c r="M25" s="72"/>
-      <c r="N25" s="72"/>
-      <c r="O25" s="72"/>
-      <c r="P25" s="73"/>
-    </row>
-    <row r="26" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D25" s="72"/>
+      <c r="E25" s="70"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="70"/>
+      <c r="J25" s="70"/>
+      <c r="K25" s="70"/>
+      <c r="L25" s="70"/>
+      <c r="M25" s="70"/>
+      <c r="N25" s="70"/>
+      <c r="O25" s="70"/>
+      <c r="P25" s="70"/>
+      <c r="Q25" s="71"/>
+    </row>
+    <row r="26" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
         <v>38</v>
       </c>
@@ -1757,11 +1784,14 @@
       <c r="O26" s="15">
         <v>12</v>
       </c>
-      <c r="P26" s="16" t="s">
+      <c r="P26" s="15">
+        <v>13</v>
+      </c>
+      <c r="Q26" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="49"/>
       <c r="B27" s="24"/>
       <c r="C27" s="24"/>
@@ -1777,12 +1807,12 @@
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
       <c r="O27" s="8"/>
-      <c r="P27" s="24"/>
-    </row>
-    <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P27" s="8"/>
+      <c r="Q27" s="24"/>
+    </row>
+    <row r="28" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="49"/>
       <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
       <c r="D28" s="25"/>
       <c r="E28" s="25"/>
       <c r="F28" s="5"/>
@@ -1795,9 +1825,10 @@
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
       <c r="O28" s="8"/>
-      <c r="P28" s="24"/>
-    </row>
-    <row r="29" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P28" s="8"/>
+      <c r="Q28" s="24"/>
+    </row>
+    <row r="29" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="49"/>
       <c r="B29" s="24"/>
       <c r="C29" s="24"/>
@@ -1813,9 +1844,10 @@
       <c r="M29" s="8"/>
       <c r="N29" s="8"/>
       <c r="O29" s="8"/>
-      <c r="P29" s="24"/>
-    </row>
-    <row r="30" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P29" s="8"/>
+      <c r="Q29" s="24"/>
+    </row>
+    <row r="30" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="49"/>
       <c r="B30" s="2"/>
       <c r="C30" s="4"/>
@@ -1831,9 +1863,10 @@
       <c r="M30" s="8"/>
       <c r="N30" s="8"/>
       <c r="O30" s="8"/>
-      <c r="P30" s="7"/>
-    </row>
-    <row r="31" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P30" s="8"/>
+      <c r="Q30" s="7"/>
+    </row>
+    <row r="31" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="49"/>
       <c r="B31" s="4"/>
       <c r="C31" s="9"/>
@@ -1849,9 +1882,10 @@
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
       <c r="O31" s="8"/>
-      <c r="P31" s="7"/>
-    </row>
-    <row r="32" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P31" s="8"/>
+      <c r="Q31" s="7"/>
+    </row>
+    <row r="32" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="49"/>
       <c r="B32" s="9"/>
       <c r="C32" s="4"/>
@@ -1867,9 +1901,10 @@
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
       <c r="O32" s="8"/>
-      <c r="P32" s="7"/>
-    </row>
-    <row r="33" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P32" s="8"/>
+      <c r="Q32" s="7"/>
+    </row>
+    <row r="33" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="49"/>
       <c r="B33" s="2"/>
       <c r="C33" s="4"/>
@@ -1885,9 +1920,10 @@
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
       <c r="O33" s="8"/>
-      <c r="P33" s="7"/>
-    </row>
-    <row r="34" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P33" s="8"/>
+      <c r="Q33" s="7"/>
+    </row>
+    <row r="34" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="49"/>
       <c r="B34" s="2"/>
       <c r="C34" s="4"/>
@@ -1903,9 +1939,10 @@
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
       <c r="O34" s="8"/>
-      <c r="P34" s="7"/>
-    </row>
-    <row r="35" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P34" s="8"/>
+      <c r="Q34" s="7"/>
+    </row>
+    <row r="35" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="49"/>
       <c r="B35" s="2"/>
       <c r="C35" s="4"/>
@@ -1921,9 +1958,10 @@
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
       <c r="O35" s="8"/>
-      <c r="P35" s="7"/>
-    </row>
-    <row r="36" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P35" s="8"/>
+      <c r="Q35" s="7"/>
+    </row>
+    <row r="36" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="50"/>
       <c r="B36" s="2"/>
       <c r="C36" s="4"/>
@@ -1939,9 +1977,10 @@
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
       <c r="O36" s="8"/>
-      <c r="P36" s="7"/>
-    </row>
-    <row r="37" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P36" s="8"/>
+      <c r="Q36" s="7"/>
+    </row>
+    <row r="37" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
@@ -1957,28 +1996,29 @@
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
+      <c r="Q37" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="25">
     <mergeCell ref="A26:A36"/>
     <mergeCell ref="A4:A8"/>
-    <mergeCell ref="D3:P3"/>
+    <mergeCell ref="D3:Q3"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="A19:A23"/>
     <mergeCell ref="A12:A18"/>
-    <mergeCell ref="D19:P23"/>
-    <mergeCell ref="D24:P24"/>
-    <mergeCell ref="D25:P25"/>
-    <mergeCell ref="D4:P8"/>
-    <mergeCell ref="D9:P11"/>
-    <mergeCell ref="D12:P15"/>
-    <mergeCell ref="D16:P18"/>
+    <mergeCell ref="D19:Q23"/>
+    <mergeCell ref="D24:Q24"/>
+    <mergeCell ref="D25:Q25"/>
+    <mergeCell ref="D4:Q8"/>
+    <mergeCell ref="D9:Q11"/>
+    <mergeCell ref="D12:Q15"/>
+    <mergeCell ref="D16:Q18"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="N1:Q1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="F2:G2"/>

</xml_diff>